<commit_message>
addressed julie's changes, and got it to 10 pages, submitting draft 1
</commit_message>
<xml_diff>
--- a/p2_sec_outcomes_kyle.xlsx
+++ b/p2_sec_outcomes_kyle.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="p2_sec_outcomes_kyle" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -681,8 +681,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="-503264576"/>
-        <c:axId val="-503269472"/>
+        <c:axId val="-772038016"/>
+        <c:axId val="-772035296"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -864,11 +864,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-503264576"/>
-        <c:axId val="-503269472"/>
+        <c:axId val="-772038016"/>
+        <c:axId val="-772035296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-503264576"/>
+        <c:axId val="-772038016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -911,7 +911,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-503269472"/>
+        <c:crossAx val="-772035296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -920,7 +920,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-503269472"/>
+        <c:axId val="-772035296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -972,7 +972,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-503264576"/>
+        <c:crossAx val="-772038016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1079,8 +1079,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="-503271648"/>
-        <c:axId val="-503263488"/>
+        <c:axId val="-772031488"/>
+        <c:axId val="-772025504"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1262,11 +1262,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-503271648"/>
-        <c:axId val="-503263488"/>
+        <c:axId val="-772031488"/>
+        <c:axId val="-772025504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-503271648"/>
+        <c:axId val="-772031488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,7 +1308,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-503263488"/>
+        <c:crossAx val="-772025504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1317,7 +1317,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-503263488"/>
+        <c:axId val="-772025504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="24"/>
@@ -1370,7 +1370,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-503271648"/>
+        <c:crossAx val="-772031488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="6"/>
@@ -1478,8 +1478,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="-503262944"/>
-        <c:axId val="-503271104"/>
+        <c:axId val="-772024960"/>
+        <c:axId val="-772028224"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1661,11 +1661,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-503262944"/>
-        <c:axId val="-503271104"/>
+        <c:axId val="-772024960"/>
+        <c:axId val="-772028224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-503262944"/>
+        <c:axId val="-772024960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1707,7 +1707,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-503271104"/>
+        <c:crossAx val="-772028224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1716,7 +1716,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-503271104"/>
+        <c:axId val="-772028224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="28"/>
@@ -1769,7 +1769,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-503262944"/>
+        <c:crossAx val="-772024960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>
@@ -5002,15 +5002,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5048,7 +5048,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5088,8 +5088,16 @@
       <c r="P2">
         <v>0</v>
       </c>
+      <c r="R2">
+        <f>AVERAGE(N2:N5)+AVERAGE(N11:N14)</f>
+        <v>17.5</v>
+      </c>
+      <c r="S2">
+        <f>AVERAGE(H2:H5)+AVERAGE(H11:H14)</f>
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -5129,8 +5137,16 @@
       <c r="P3">
         <v>1</v>
       </c>
+      <c r="R3">
+        <f>AVERAGE(N6:N10)+AVERAGE(N15:N21)</f>
+        <v>17.085714285714289</v>
+      </c>
+      <c r="S3">
+        <f>AVERAGE(H6:H10) + AVERAGE(H15:H21)</f>
+        <v>15.8</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -5170,8 +5186,16 @@
       <c r="P4">
         <v>2</v>
       </c>
+      <c r="R4">
+        <f>R2-R3</f>
+        <v>0.41428571428571104</v>
+      </c>
+      <c r="S4">
+        <f>S2-S3</f>
+        <v>0.19999999999999929</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -5212,7 +5236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -5262,7 +5286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -5303,7 +5327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -5344,7 +5368,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -5385,7 +5409,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -5426,7 +5450,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -5476,7 +5500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -5517,7 +5541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -5558,7 +5582,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -5599,7 +5623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -5649,7 +5673,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>

</xml_diff>